<commit_message>
Update table with reversible and fast #3
</commit_message>
<xml_diff>
--- a/data/manual_curation.xlsx
+++ b/data/manual_curation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_GEMs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F905510-0937-2744-86F2-3DF7CAB454E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18F63E35-CAEA-D143-A9E8-05AB34E80A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="28940" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metab" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="296">
   <si>
     <t>BIGG</t>
   </si>
@@ -816,9 +816,6 @@
     <t>pan4p_c</t>
   </si>
   <si>
-    <t>ATP:pantetheine 4'-phosphotransferase</t>
-  </si>
-  <si>
     <t>RHEA</t>
   </si>
   <si>
@@ -846,9 +843,6 @@
     <t>APCPT</t>
   </si>
   <si>
-    <t>ATP:pantothenoyl-L-cysteine 4'-phosphotransferase</t>
-  </si>
-  <si>
     <t>ptcys_c</t>
   </si>
   <si>
@@ -898,6 +892,24 @@
   </si>
   <si>
     <t>sbo</t>
+  </si>
+  <si>
+    <t>fast</t>
+  </si>
+  <si>
+    <t>ATP:pantetheine 4-phosphotransferase</t>
+  </si>
+  <si>
+    <t>ATP:pantothenoyl-L-cysteine 4-phosphotransferase</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>reversible</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -976,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1005,9 +1017,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1316,7 +1325,7 @@
   </sheetPr>
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
@@ -3248,19 +3257,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35DF402-707E-F145-925A-05F806C63C3A}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="21.1640625" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" customWidth="1"/>
+    <col min="8" max="9" width="21.1640625" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -3277,42 +3286,47 @@
         <v>258</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>251</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="J1" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>269</v>
-      </c>
       <c r="N1" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="T1" s="10"/>
-    </row>
-    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="U1" s="10"/>
+    </row>
+    <row r="2" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>256</v>
       </c>
@@ -3328,38 +3342,44 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>288</v>
+      <c r="F2" s="12" t="s">
+        <v>286</v>
       </c>
       <c r="G2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H2" t="s">
-        <v>264</v>
-      </c>
-      <c r="I2">
+        <v>291</v>
+      </c>
+      <c r="I2" t="s">
+        <v>295</v>
+      </c>
+      <c r="J2" t="s">
+        <v>293</v>
+      </c>
+      <c r="K2">
         <v>22472</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
+        <v>265</v>
+      </c>
+      <c r="M2" t="s">
         <v>266</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>267</v>
       </c>
-      <c r="L2" t="s">
-        <v>268</v>
-      </c>
-      <c r="M2" t="s">
-        <v>271</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>270</v>
       </c>
       <c r="P2" t="s">
+        <v>269</v>
+      </c>
+      <c r="R2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>256</v>
       </c>
@@ -3375,14 +3395,14 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>22473</v>
       </c>
-      <c r="M3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>256</v>
       </c>
@@ -3392,21 +3412,21 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>22474</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>256</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>22475</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B6" t="s">
         <v>259</v>
@@ -3415,42 +3435,48 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>288</v>
+      <c r="F6" s="12" t="s">
+        <v>286</v>
       </c>
       <c r="G6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H6" t="s">
-        <v>274</v>
+        <v>292</v>
+      </c>
+      <c r="I6" t="s">
+        <v>295</v>
       </c>
       <c r="J6" t="s">
-        <v>278</v>
-      </c>
-      <c r="K6" t="s">
+        <v>293</v>
+      </c>
+      <c r="L6" t="s">
+        <v>276</v>
+      </c>
+      <c r="M6" t="s">
+        <v>275</v>
+      </c>
+      <c r="O6" t="s">
+        <v>270</v>
+      </c>
+      <c r="P6" t="s">
         <v>277</v>
       </c>
-      <c r="M6" t="s">
-        <v>271</v>
-      </c>
-      <c r="N6" t="s">
-        <v>279</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" t="s">
         <v>273</v>
-      </c>
-      <c r="B7" t="s">
-        <v>275</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3462,9 +3488,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" t="s">
         <v>262</v>
@@ -3490,16 +3516,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C1">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -3507,13 +3533,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3521,7 +3547,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Append table with more research #3
</commit_message>
<xml_diff>
--- a/data/manual_curation.xlsx
+++ b/data/manual_curation.xlsx
@@ -1,28 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_GEMs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18F63E35-CAEA-D143-A9E8-05AB34E80A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938C40BF-145B-EF4B-9768-FDB3534D47A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="28940" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28940" windowHeight="14100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metab" sheetId="1" r:id="rId1"/>
     <sheet name="gapfill" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="301">
   <si>
     <t>BIGG</t>
   </si>
@@ -910,13 +922,28 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>NP1</t>
+  </si>
+  <si>
+    <t>falsch rum laut model seed sollte die anders rum sein</t>
+  </si>
+  <si>
+    <t>NT5C</t>
+  </si>
+  <si>
+    <t>https://www.genome.jp/entry/cstr:CBE89_06525</t>
+  </si>
+  <si>
+    <t>: WP_086891288</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -960,6 +987,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -985,10 +1020,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1018,8 +1054,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1325,7 +1363,7 @@
   </sheetPr>
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
@@ -3506,15 +3544,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFB7E9A-9815-E24C-AE11-98E2601D71AD}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>282</v>
       </c>
@@ -3531,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>279</v>
       </c>
@@ -3545,12 +3583,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>283</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>298</v>
+      </c>
+      <c r="F9" t="s">
+        <v>299</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1" tooltip="Show report for WP_086891288.1" display="https://www.ncbi.nlm.nih.gov/protein/WP_086891288.1?report=genbank&amp;log$=protalign&amp;blast_rank=1&amp;RID=DMV906J201R" xr:uid="{BC2A3DF0-DAB1-DF4C-99BD-63D54D643D65}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>